<commit_message>
modificacion para tesoreria y comercializacion
</commit_message>
<xml_diff>
--- a/storage/ExtractoPago.xlsx
+++ b/storage/ExtractoPago.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>FECHA</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>CALLE LIMACO ALDAIR</t>
+  </si>
+  <si>
+    <t>ACOSTA SAAVEDRA MARIA SOLEDAD</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:H29"/>
+      <selection activeCell="A1" sqref="A1:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -497,7 +500,7 @@
     <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="38.847656" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="29.421387" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="35.2771" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="54.129639" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="28.135986" bestFit="true" customWidth="true" style="0"/>
@@ -1254,6 +1257,32 @@
         <v>30.0</v>
       </c>
       <c r="H29" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2">
+        <v>12200</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="2">
+        <v>17</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
base de datos vacia con las modificaciones para prueba
</commit_message>
<xml_diff>
--- a/storage/ExtractoPago.xlsx
+++ b/storage/ExtractoPago.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>NOMBRE DE RUBRO</t>
   </si>
@@ -81,6 +81,30 @@
     <t>Certificados de Notas  nivel Tecnico Superior</t>
   </si>
   <si>
+    <t>Historicos academicos</t>
+  </si>
+  <si>
+    <t>2021-05-10</t>
+  </si>
+  <si>
+    <t>DIPLOMA ACADEMICO DE DIPLOMADO</t>
+  </si>
+  <si>
+    <t>2021-05-11</t>
+  </si>
+  <si>
+    <t>Producto Avicola2</t>
+  </si>
+  <si>
+    <t>Pago de Alevines</t>
+  </si>
+  <si>
+    <t>2021-05-17</t>
+  </si>
+  <si>
+    <t>2021-05-18</t>
+  </si>
+  <si>
     <t>Vice Rectorado</t>
   </si>
   <si>
@@ -90,66 +114,6 @@
   </si>
   <si>
     <t>pago de certificados de notas</t>
-  </si>
-  <si>
-    <t>Historicos academicos</t>
-  </si>
-  <si>
-    <t>2021-05-10</t>
-  </si>
-  <si>
-    <t>DIPLOMA ACADEMICO DE DIPLOMADO</t>
-  </si>
-  <si>
-    <t>2021-05-11</t>
-  </si>
-  <si>
-    <t>Producto Avicola2</t>
-  </si>
-  <si>
-    <t>Pago de Alevines</t>
-  </si>
-  <si>
-    <t>2021-05-17</t>
-  </si>
-  <si>
-    <t>2021-05-18</t>
-  </si>
-  <si>
-    <t>2023-08-11</t>
-  </si>
-  <si>
-    <t>2023-08-14</t>
-  </si>
-  <si>
-    <t>2023-08-28</t>
-  </si>
-  <si>
-    <t>Externa</t>
-  </si>
-  <si>
-    <t>Derechos</t>
-  </si>
-  <si>
-    <t>Almacenes</t>
-  </si>
-  <si>
-    <t>pollos</t>
-  </si>
-  <si>
-    <t>Interna</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>Medicina Veterinaria y Zootecnia</t>
-  </si>
-  <si>
-    <t>Perejil</t>
-  </si>
-  <si>
-    <t>2023-08-31</t>
   </si>
 </sst>
 </file>
@@ -529,22 +493,22 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:K53"/>
+      <selection activeCell="A1" sqref="A1:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="38.848" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="54.13" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="6.998" bestFit="true" customWidth="true" style="0"/>
@@ -978,13 +942,11 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E14" s="2">
         <v>7</v>
@@ -1000,10 +962,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="2">
-        <v>30.0</v>
+        <v>15.0</v>
       </c>
       <c r="K14" s="2">
-        <v>30.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1015,10 +977,10 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
@@ -1044,15 +1006,17 @@
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -1062,10 +1026,10 @@
         <v>1</v>
       </c>
       <c r="J16" s="2">
-        <v>15.0</v>
+        <v>200.0</v>
       </c>
       <c r="K16" s="2">
-        <v>15.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1073,19 +1037,17 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="2">
-        <v>8</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
@@ -1108,17 +1070,15 @@
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -1128,10 +1088,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="2">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
       <c r="K18" s="2">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1141,15 +1101,17 @@
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -1159,10 +1121,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="2">
-        <v>30.0</v>
+        <v>200.0</v>
       </c>
       <c r="K19" s="2">
-        <v>30.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1174,13 +1136,13 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E20" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
@@ -1190,10 +1152,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="2">
-        <v>30.0</v>
+        <v>300.0</v>
       </c>
       <c r="K20" s="2">
-        <v>30.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1204,26 +1166,26 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E21" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J21" s="2">
-        <v>200.0</v>
+        <v>2.0</v>
       </c>
       <c r="K21" s="2">
         <v>200.0</v>
@@ -1236,15 +1198,17 @@
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
@@ -1254,10 +1218,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="2">
-        <v>300.0</v>
+        <v>2.0</v>
       </c>
       <c r="K22" s="2">
-        <v>300.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1268,29 +1232,29 @@
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="2">
-        <v>3</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J23" s="2">
         <v>2.0</v>
       </c>
       <c r="K23" s="2">
-        <v>200.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1301,16 +1265,16 @@
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="2">
-        <v>4</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
@@ -1333,17 +1297,15 @@
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
@@ -1353,10 +1315,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="2">
-        <v>2.0</v>
+        <v>15.0</v>
       </c>
       <c r="K25" s="2">
-        <v>2.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1367,16 +1329,16 @@
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
@@ -1386,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="J26" s="2">
-        <v>2.0</v>
+        <v>200.0</v>
       </c>
       <c r="K26" s="2">
-        <v>2.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1399,15 +1361,17 @@
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E27" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
@@ -1417,10 +1381,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="2">
-        <v>15.0</v>
+        <v>2.0</v>
       </c>
       <c r="K27" s="2">
-        <v>15.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1428,19 +1392,19 @@
         <v>11</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E28" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G28" s="2">
         <v>0</v>
@@ -1450,10 +1414,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="2">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
       <c r="K28" s="2">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1461,19 +1425,19 @@
         <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E29" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G29" s="2">
         <v>0</v>
@@ -1494,19 +1458,19 @@
         <v>11</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="2">
+        <v>7</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="2">
-        <v>8</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
@@ -1516,783 +1480,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="2">
-        <v>2.0</v>
+        <v>30.0</v>
       </c>
       <c r="K30" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="2">
-        <v>9</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K31" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="2">
-        <v>10</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2">
-        <v>300.0</v>
-      </c>
-      <c r="K32" s="2">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="2">
-        <v>10</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K33" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="2">
-        <v>10</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="2">
-        <v>0</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2">
-        <v>1</v>
-      </c>
-      <c r="J34" s="2">
-        <v>15.0</v>
-      </c>
-      <c r="K34" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="2">
-        <v>11</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G35" s="2">
-        <v>0</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2">
-        <v>1</v>
-      </c>
-      <c r="J35" s="2">
         <v>30.0</v>
-      </c>
-      <c r="K35" s="2">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="2">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" s="2">
-        <v>1</v>
-      </c>
-      <c r="J36" s="2">
-        <v>15.0</v>
-      </c>
-      <c r="K36" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="2">
-        <v>11</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="2">
-        <v>1</v>
-      </c>
-      <c r="J37" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="K37" s="2">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="2">
-        <v>12</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="2">
-        <v>0</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I38" s="2">
-        <v>1</v>
-      </c>
-      <c r="J38" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K38" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="2">
-        <v>12</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="2">
-        <v>1234</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I39" s="2">
-        <v>1</v>
-      </c>
-      <c r="J39" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="K39" s="2">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="2">
-        <v>13</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="2">
-        <v>0</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I40" s="2">
-        <v>1</v>
-      </c>
-      <c r="J40" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K40" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="2">
-        <v>14</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="2">
-        <v>0</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" s="2">
-        <v>1</v>
-      </c>
-      <c r="J41" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K41" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="2">
-        <v>13</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G42" s="2">
-        <v>0</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I42" s="2">
-        <v>1</v>
-      </c>
-      <c r="J42" s="2">
-        <v>15.0</v>
-      </c>
-      <c r="K42" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="2">
-        <v>14</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="2">
-        <v>12345</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I43" s="2">
-        <v>1</v>
-      </c>
-      <c r="J43" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K43" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="2">
-        <v>15</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G44" s="2">
-        <v>0</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I44" s="2">
-        <v>1</v>
-      </c>
-      <c r="J44" s="2">
-        <v>200.0</v>
-      </c>
-      <c r="K44" s="2">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="2">
-        <v>16</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G45" s="2">
-        <v>0</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="2">
-        <v>1</v>
-      </c>
-      <c r="J45" s="2">
-        <v>15.0</v>
-      </c>
-      <c r="K45" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="2">
-        <v>15</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G46" s="2">
-        <v>741</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I46" s="2">
-        <v>1</v>
-      </c>
-      <c r="J46" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="K46" s="2">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E47" s="2">
-        <v>16</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G47" s="2">
-        <v>0</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I47" s="2">
-        <v>1</v>
-      </c>
-      <c r="J47" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="K47" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" s="2">
-        <v>17</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G48" s="2">
-        <v>4545</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I48" s="2">
-        <v>1</v>
-      </c>
-      <c r="J48" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K48" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="2">
-        <v>18</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G49" s="2">
-        <v>12345</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I49" s="2">
-        <v>2</v>
-      </c>
-      <c r="J49" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="K49" s="2">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E50" s="2">
-        <v>18</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G50" s="2">
-        <v>12345</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I50" s="2">
-        <v>2</v>
-      </c>
-      <c r="J50" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K50" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E51" s="2">
-        <v>19</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G51" s="2">
-        <v>0</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I51" s="2">
-        <v>1</v>
-      </c>
-      <c r="J51" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="K51" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" s="2">
-        <v>20</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G52" s="2">
-        <v>0</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I52" s="2">
-        <v>1</v>
-      </c>
-      <c r="J52" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="K52" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E53" s="2">
-        <v>21</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G53" s="2">
-        <v>7898</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I53" s="2">
-        <v>1</v>
-      </c>
-      <c r="J53" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="K53" s="2">
-        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>